<commit_message>
implemented dep ttest, improved documentation
</commit_message>
<xml_diff>
--- a/dataPublic/pooledData_forAlansProject.xlsx
+++ b/dataPublic/pooledData_forAlansProject.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\ZlabCode\qtProjects\autograph_behavior\dataPublic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59646824-F6E5-43D7-AAEA-69BC0122155B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B360EA74-C363-4886-9765-E567B0E5CD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-16335" windowWidth="29040" windowHeight="16440" xr2:uid="{8B3003D0-32F9-48A0-8C92-7F37FB6AAB52}"/>
+    <workbookView xWindow="-28920" yWindow="5310" windowWidth="29040" windowHeight="16440" xr2:uid="{8B3003D0-32F9-48A0-8C92-7F37FB6AAB52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -573,25 +573,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56758F5D-BD9A-45D6-AB54-39B75D115899}">
   <dimension ref="A1:W68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.7890625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.3125" customWidth="1"/>
-    <col min="3" max="3" width="18.9453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83984375" customWidth="1"/>
-    <col min="6" max="6" width="16.05078125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.1015625" customWidth="1"/>
-    <col min="9" max="9" width="16.26171875" customWidth="1"/>
-    <col min="10" max="10" width="15.1015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -622,7 +622,7 @@
       <c r="P1" s="2"/>
       <c r="W1" s="2"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -652,7 +652,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -682,7 +682,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -712,7 +712,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -742,7 +742,7 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -772,7 +772,7 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -802,7 +802,7 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -832,7 +832,7 @@
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -862,7 +862,7 @@
       </c>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -892,7 +892,7 @@
       </c>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -922,7 +922,7 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -952,7 +952,7 @@
       </c>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -982,7 +982,7 @@
       </c>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1012,7 +1012,7 @@
       </c>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1042,7 +1042,7 @@
       </c>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1072,7 +1072,7 @@
       </c>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1132,7 +1132,7 @@
       </c>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1162,7 +1162,7 @@
       </c>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1282,7 +1282,7 @@
       </c>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1312,7 +1312,7 @@
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1402,7 +1402,7 @@
       </c>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1462,7 +1462,7 @@
       </c>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -1492,7 +1492,7 @@
       </c>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -1552,7 +1552,7 @@
       </c>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -1612,7 +1612,7 @@
       </c>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -1672,7 +1672,7 @@
       </c>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -1702,79 +1702,79 @@
       </c>
       <c r="J37" s="1"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B45" s="4"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C47" s="2"/>
     </row>
-    <row r="49" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
     </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
     </row>
-    <row r="54" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
     </row>
-    <row r="55" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
     </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
     </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
     </row>
-    <row r="59" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C68" s="2"/>
     </row>
   </sheetData>

</xml_diff>